<commit_message>
List all the items we intend to put in the welcome kit, plus additional resources.
</commit_message>
<xml_diff>
--- a/track and report.xlsx
+++ b/track and report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>How to use this workbook</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Familiarize yourself with this workbook. If you do iterative planning, planning &amp; scheduling happens on the Plan sheet. Tracking / data entry will happen on the Data sheet. Reporting / results are split between the Dashboard (visualizations that help you course-correct based on current data) and Historical trends (visualizations that help you see how the team has changed over time).</t>
+  </si>
+  <si>
+    <t>Demo date</t>
   </si>
 </sst>
 </file>
@@ -587,10 +590,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Now with a form of tracking that handles both continuous-form and iterative planning. Just record a date and the deltas since the last date. Also defines & color-codes the 4 kinds of work. Will use consistent colors throughout, setting up a visual metaphor that people can use as a shorthand across the company (blue work, purple work, etc)
</commit_message>
<xml_diff>
--- a/track and report.xlsx
+++ b/track and report.xlsx
@@ -4,22 +4,393 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Readme - how to use" sheetId="1" r:id="rId1"/>
     <sheet name="Dashboard" sheetId="2" r:id="rId2"/>
     <sheet name="Historical trends" sheetId="3" r:id="rId3"/>
-    <sheet name="Plan" sheetId="6" r:id="rId4"/>
-    <sheet name="Data" sheetId="4" r:id="rId5"/>
-    <sheet name="Settings" sheetId="5" r:id="rId6"/>
+    <sheet name="Data" sheetId="4" r:id="rId4"/>
+    <sheet name="Calcs" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+All columns except Date are story card counts.
+Blue work items are product work improvements. This means they relate to any aspect of the business's product and we have evidence that they implement the right solution to an important problem.
+Their purpose is to realize value, turning our knowledge of the customer into product advantage.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cards added to the near-future plan, such as the sprint commitment or the ready for work queue.
+These represent the planned objectives, either strategic or tactical.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cards added to work that bypassed the planning cycle, such as during-sprint adds to the sprint or urgent work that bypasses the ready queue and takes the urgent item swimlane.
+Special note: bugs should always be added additional work, even if they are later removed or were known at the sprint start. Bugs are never planned work, even if they were triaged and scheduled.
+Bugs are also always product improvements (blue work). A bug fix is never an experiment (you know the value), and it is never a sustainability item (an action taken to prevent a certain category of bug from ever happening again would be a sustainability item).
+Your team needs to agree about what a bug means. But think of it in terms of measurability. A bug means that a story or part of a story, while bellieved to be done, was done in such a way that the measures of impact don't actually assess the worth of the idea - something gets in the way and changes user behavior. This means that the team has to do additional work in order for the system to actually measure impact of the stories in question.
+These represent additional work the team has to do that do not further its plan, such as bug fixes, emergencies, special projects, or overhead.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Work items that are removed from the plan without being done.
+These aren't just delayed until later. Instead, the team decides to not do them. They are no longer intended to be part of the product.
+Note: all items here are planned work only. Don't record additional adds that were removed without being done. Just take those out of the added additional as if they were never there. If you did partial progress on an added work item and then dropped the rest, consider it as completed additional work.
+They represent places where the team has gained information that allowed them to realize some work would not be worth doing, and then make the choice to not do that work.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Completed work items that were planned (as in, showed up in the added to plan column at some point in the past and were never removed).
+These represent progress towards the planned objectives for the product.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Completed work items that bypassed the plan.
+These represent effort expended that did not accrue to the planned objectives.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Work items that were neither completed nor removed. It will be carried over into the future, into the backlog for future plans.
+Note: the work should balance for any period. The amount of work taken into the immediate-term plan - (done + removed from plan + remaining) should be zero. Use this to check that you didn't miss anything.
+This represents work that is not yet done, but we intend to do some day.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Stories that were not only completed, but had the expected impact.
+This is not about acceptance criteria. Acceptance criteria tell you when a story is done: those allow a story to be added to the done columns.
+This is about impact criteria: how did the story impact the customer behavior? Frequently we will do good work that does what we intend, but it will have different custommer impacts than we had hoped. This column represents stories that had the measurable impact that we had hoped for.
+This represents actual value accrual for the company. The story materially changed the company's revenue or revenue-leading measures.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+All columns except Date are story card counts.
+Green work items are product work experiments. This means they relate to any aspect of the business's product and we know what problem they are trying to solve, but don't have evidence yet what solution will best address that problem.
+Their purpose is to try out a potential solution and gain information about what works.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cards added to the near-future plan, such as the sprint commitment or the ready for work queue.
+These represent the planned objectives, either strategic or tactical.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+All columns except Date are story card counts.
+Purple work items are sustainabillity work improvements. This means they relate to any aspect of improving your capacity to do business and we have evidence that they implement the right solution to an important problem.
+Their purpose is to realize a process or habit change, turning our knowledge of the system into a business advantage.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cards added to the near-future plan, such as the sprint commitment or the ready for work queue.
+These represent the planned objectives, either strategic or tactical.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+All columns except Date are story card counts.
+Orange work items are sustainability work experiments. This means they relate to any aspect of the team's capacity to do business and we know what problem they are trying to solve, but don't have evidence yet what solution will best address that problem.
+Their purpose is to try out a potential solution and gain information about what works.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cards added to the near-future plan, such as the sprint commitment or the ready for work queue.
+These represent the planned objectives, either strategic or tactical.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>How to use this workbook</t>
   </si>
@@ -54,38 +425,92 @@
     <t>Right before planning meeting: determine your available capacity (see plannning sheet). This is based on your budget - the spending ratio between product and sustainability stories.</t>
   </si>
   <si>
-    <t>This team uses regularly-scheduled, recurring planning meetings:</t>
-  </si>
-  <si>
     <t>Assumptions: your team uses a recurring, regularly-scheduled demo for product work. Your team will do the same for sustainability work. Your planning may be iterative or continuous-form, but demos happen on a cadence.</t>
   </si>
   <si>
-    <t>First product demo date</t>
-  </si>
-  <si>
-    <t>Product demo cycle length (in workdays)</t>
-  </si>
-  <si>
-    <t>First sustainability demo date</t>
-  </si>
-  <si>
-    <t>Sustainability demo cycle length (in workdays)</t>
-  </si>
-  <si>
-    <t>If so, number of workdays between demo and the next plan</t>
-  </si>
-  <si>
     <t>Familiarize yourself with this workbook. If you do iterative planning, planning &amp; scheduling happens on the Plan sheet. Tracking / data entry will happen on the Data sheet. Reporting / results are split between the Dashboard (visualizations that help you course-correct based on current data) and Historical trends (visualizations that help you see how the team has changed over time).</t>
   </si>
   <si>
-    <t>Demo date</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Additional done</t>
+  </si>
+  <si>
+    <t>Planned done</t>
+  </si>
+  <si>
+    <t>Removed</t>
+  </si>
+  <si>
+    <t>Had expected impact</t>
+  </si>
+  <si>
+    <t>Product Improvements</t>
+  </si>
+  <si>
+    <t>Product Experiments</t>
+  </si>
+  <si>
+    <t>Sustainability Improvements</t>
+  </si>
+  <si>
+    <t>Sustainability Experiments</t>
+  </si>
+  <si>
+    <t>Added Additional</t>
+  </si>
+  <si>
+    <t>Carried Over</t>
+  </si>
+  <si>
+    <t>Sustain percentage goal</t>
+  </si>
+  <si>
+    <t>Chart with actuals over recent time</t>
+  </si>
+  <si>
+    <t>as small table with date and goal</t>
+  </si>
+  <si>
+    <t>Actual % with impact, for the two improvement colors, with control band</t>
+  </si>
+  <si>
+    <t>Actual % with impact, for the two experiment colors, with control band</t>
+  </si>
+  <si>
+    <t>Target number of experiment options to run</t>
+  </si>
+  <si>
+    <t>Especially note the special note about bugs. Bugs are always blue work, and are always additional added items (not planned work). This is true whether they were triaged (delayed until future planning) or not.</t>
+  </si>
+  <si>
+    <t>Actual % implemented, for each of the 4 colors on one chart</t>
+  </si>
+  <si>
+    <t>Actual total work done, for each color, showing planned and total</t>
+  </si>
+  <si>
+    <t>Current percentage of work going to planned work, per color</t>
+  </si>
+  <si>
+    <t>Taken into Immediate Future Plan</t>
+  </si>
+  <si>
+    <t>CFD with short- and long- term plan work, improvements only</t>
+  </si>
+  <si>
+    <t>Remaining Planned</t>
+  </si>
+  <si>
+    <t>Removed Planned</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,13 +533,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -135,12 +608,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -151,14 +628,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
+    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
+    <cellStyle name="Accent3" xfId="4" builtinId="37"/>
+    <cellStyle name="Accent4" xfId="5" builtinId="41"/>
+    <cellStyle name="Accent6" xfId="6" builtinId="49"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -169,6 +674,110 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="actuals_prd_imp" displayName="actuals_prd_imp" ref="B1:I1048576" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="B1:I1048576">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Date"/>
+    <tableColumn id="2" name="Taken into Immediate Future Plan"/>
+    <tableColumn id="3" name="Added Additional"/>
+    <tableColumn id="4" name="Removed Planned"/>
+    <tableColumn id="5" name="Planned done"/>
+    <tableColumn id="6" name="Additional done"/>
+    <tableColumn id="8" name="Remaining Planned"/>
+    <tableColumn id="7" name="Had expected impact"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="actuals_prd_exp" displayName="actuals_prd_exp" ref="K1:R1048576" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="K1:R1048576">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Date"/>
+    <tableColumn id="2" name="Taken into Immediate Future Plan"/>
+    <tableColumn id="3" name="Added Additional"/>
+    <tableColumn id="4" name="Removed"/>
+    <tableColumn id="5" name="Planned done"/>
+    <tableColumn id="6" name="Additional done"/>
+    <tableColumn id="8" name="Carried Over"/>
+    <tableColumn id="7" name="Had expected impact"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="actuals_stn_exp" displayName="actuals_stn_exp" ref="AC1:AJ1048576" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="AC1:AJ1048576">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Date"/>
+    <tableColumn id="2" name="Taken into Immediate Future Plan"/>
+    <tableColumn id="3" name="Added Additional"/>
+    <tableColumn id="4" name="Removed"/>
+    <tableColumn id="5" name="Planned done"/>
+    <tableColumn id="6" name="Additional done"/>
+    <tableColumn id="8" name="Carried Over"/>
+    <tableColumn id="7" name="Had expected impact"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="actuals_stn_imp" displayName="actuals_stn_imp" ref="T1:AA1048576" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="T1:AA1048576">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Date"/>
+    <tableColumn id="2" name="Taken into Immediate Future Plan"/>
+    <tableColumn id="3" name="Added Additional"/>
+    <tableColumn id="4" name="Removed"/>
+    <tableColumn id="5" name="Planned done"/>
+    <tableColumn id="6" name="Additional done"/>
+    <tableColumn id="8" name="Carried Over"/>
+    <tableColumn id="7" name="Had expected impact"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,7 +1090,7 @@
     </row>
     <row r="3" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="20" thickBot="1" x14ac:dyDescent="0.5">
@@ -501,46 +1110,51 @@
     </row>
     <row r="7" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:1" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:1" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:1" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:1" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -551,6 +1165,343 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D2:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" customWidth="1"/>
+    <col min="7" max="8" width="16.08984375" customWidth="1"/>
+    <col min="9" max="9" width="20.26953125" customWidth="1"/>
+    <col min="12" max="12" width="13.08984375" customWidth="1"/>
+    <col min="13" max="13" width="10.26953125" customWidth="1"/>
+    <col min="14" max="14" width="10.6328125" customWidth="1"/>
+    <col min="15" max="15" width="14.26953125" customWidth="1"/>
+    <col min="16" max="17" width="16.08984375" customWidth="1"/>
+    <col min="18" max="18" width="20.26953125" customWidth="1"/>
+    <col min="21" max="21" width="13.7265625" customWidth="1"/>
+    <col min="22" max="22" width="11.54296875" customWidth="1"/>
+    <col min="23" max="23" width="10.6328125" customWidth="1"/>
+    <col min="24" max="24" width="14.26953125" customWidth="1"/>
+    <col min="25" max="26" width="16.08984375" customWidth="1"/>
+    <col min="27" max="27" width="20.26953125" customWidth="1"/>
+    <col min="30" max="30" width="13.1796875" customWidth="1"/>
+    <col min="31" max="31" width="11.36328125" customWidth="1"/>
+    <col min="32" max="32" width="10.6328125" customWidth="1"/>
+    <col min="33" max="33" width="14.26953125" customWidth="1"/>
+    <col min="34" max="35" width="16.08984375" customWidth="1"/>
+    <col min="36" max="36" width="20.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A2" s="4"/>
+      <c r="J2" s="5"/>
+      <c r="S2" s="6"/>
+      <c r="AB2" s="7"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="J3" s="5"/>
+      <c r="S3" s="6"/>
+      <c r="AB3" s="7"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="J4" s="5"/>
+      <c r="S4" s="6"/>
+      <c r="AB4" s="7"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="J5" s="5"/>
+      <c r="S5" s="6"/>
+      <c r="AB5" s="7"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="J6" s="5"/>
+      <c r="S6" s="6"/>
+      <c r="AB6" s="7"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="J7" s="5"/>
+      <c r="S7" s="6"/>
+      <c r="AB7" s="7"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="J8" s="5"/>
+      <c r="S8" s="6"/>
+      <c r="AB8" s="7"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A9" s="4"/>
+      <c r="J9" s="5"/>
+      <c r="S9" s="6"/>
+      <c r="AB9" s="7"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A10" s="4"/>
+      <c r="J10" s="5"/>
+      <c r="S10" s="6"/>
+      <c r="AB10" s="7"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A11" s="4"/>
+      <c r="J11" s="5"/>
+      <c r="S11" s="6"/>
+      <c r="AB11" s="7"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A12" s="4"/>
+      <c r="J12" s="5"/>
+      <c r="S12" s="6"/>
+      <c r="AB12" s="7"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A13" s="4"/>
+      <c r="J13" s="5"/>
+      <c r="S13" s="6"/>
+      <c r="AB13" s="7"/>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="J14" s="5"/>
+      <c r="S14" s="6"/>
+      <c r="AB14" s="7"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="J15" s="5"/>
+      <c r="S15" s="6"/>
+      <c r="AB15" s="7"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="J16" s="5"/>
+      <c r="S16" s="6"/>
+      <c r="AB16" s="7"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A17" s="4"/>
+      <c r="J17" s="5"/>
+      <c r="S17" s="6"/>
+      <c r="AB17" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A17"/>
+    <mergeCell ref="J1:J17"/>
+    <mergeCell ref="S1:S17"/>
+    <mergeCell ref="AB1:AB17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <tableParts count="4">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -560,114 +1511,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="43.81640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4">
-        <v>42522</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="4">
-        <v>42522</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>